<commit_message>
Implementacion Asignacion 10 y unos ajustes al proyecto final.
</commit_message>
<xml_diff>
--- a/ProyectosUnidad4/Para probar métodos.xlsx
+++ b/ProyectosUnidad4/Para probar métodos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miawlucii\Documents\GitHub\ProyectosMatematicas\ProyectosUnidad4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E65060-50EA-4324-87F8-9EDCFB48DC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D936EC37-7CB4-4E66-9B0C-6F4410B1593E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29C1A40B-E894-4306-922C-CA8E46BC1C48}"/>
   </bookViews>
@@ -458,15 +458,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74A4687-6D7F-44D3-B214-E99A0A126C6F}">
-  <dimension ref="E2:P15"/>
+  <dimension ref="E2:Z18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -480,7 +480,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -494,7 +494,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
@@ -516,7 +516,7 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E5" s="1">
         <v>1</v>
       </c>
@@ -547,8 +547,29 @@
       <c r="P5" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>9.9</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>1.2</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>2</v>
       </c>
@@ -579,8 +600,29 @@
       <c r="P6" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>9</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>0.6</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="7" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>3</v>
       </c>
@@ -611,8 +653,29 @@
       <c r="P7" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>8.1</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="V7">
+        <v>0.4</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="8" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>4</v>
       </c>
@@ -643,8 +706,29 @@
       <c r="P8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>7.1</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+      <c r="V8">
+        <v>-0.2</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <v>2</v>
+      </c>
+      <c r="Z8">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="9" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>5</v>
       </c>
@@ -675,8 +759,29 @@
       <c r="P9" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>6.2</v>
+      </c>
+      <c r="U9">
+        <v>9</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>3</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>6</v>
       </c>
@@ -707,8 +812,29 @@
       <c r="P10" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>5.3</v>
+      </c>
+      <c r="U10">
+        <v>11</v>
+      </c>
+      <c r="V10">
+        <v>-0.6</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <v>2</v>
+      </c>
+      <c r="Z10">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="11" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
         <v>7</v>
       </c>
@@ -725,8 +851,29 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>7</v>
+      </c>
+      <c r="S11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="U11">
+        <v>13</v>
+      </c>
+      <c r="V11">
+        <v>-0.4</v>
+      </c>
+      <c r="X11">
+        <v>4</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="12" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -739,8 +886,29 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>8</v>
+      </c>
+      <c r="S12">
+        <v>3.6</v>
+      </c>
+      <c r="U12">
+        <v>15</v>
+      </c>
+      <c r="V12">
+        <v>-0.2</v>
+      </c>
+      <c r="X12">
+        <v>4</v>
+      </c>
+      <c r="Y12">
+        <v>2</v>
+      </c>
+      <c r="Z12">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -753,8 +921,20 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>9</v>
+      </c>
+      <c r="S13">
+        <v>2.7</v>
+      </c>
+      <c r="U13">
+        <v>17</v>
+      </c>
+      <c r="V13">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -767,8 +947,20 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <v>1.8</v>
+      </c>
+      <c r="U14">
+        <v>19</v>
+      </c>
+      <c r="V14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="5:26" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -781,6 +973,48 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
+      <c r="R15">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>23</v>
+      </c>
+      <c r="V15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>12</v>
+      </c>
+      <c r="S16">
+        <v>-0.7</v>
+      </c>
+      <c r="U16">
+        <v>25</v>
+      </c>
+      <c r="V16">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="17" spans="18:19" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>13</v>
+      </c>
+      <c r="S17">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="18:19" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>14</v>
+      </c>
+      <c r="S18">
+        <v>-2.2999999999999998</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>